<commit_message>
consistent format for input data
</commit_message>
<xml_diff>
--- a/import_data/example_labels.xlsx
+++ b/import_data/example_labels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janbode/dxp/backend/import_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janbode/ladder.ly/import_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7199C186-4C76-0243-8367-AD27D50E39B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B690A3-7F5F-5B49-830E-66173224852A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7280" yWindow="1340" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Sense of Comfort</t>
-  </si>
-  <si>
-    <t>labels</t>
   </si>
   <si>
     <t>Sharing Information and Data</t>
@@ -429,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -442,52 +439,55 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -503,7 +503,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -511,7 +511,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -519,47 +519,47 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -567,7 +567,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -575,49 +575,33 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>